<commit_message>
Add provantage price pull. Clean folder structure. Debug text.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Newegg" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="PCM" sheetId="4" r:id="rId4"/>
     <sheet name="Insight" sheetId="5" r:id="rId5"/>
     <sheet name="Zones" sheetId="6" r:id="rId6"/>
+    <sheet name="Provantage" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Links</t>
   </si>
@@ -78,7 +79,22 @@
     <t>65SE3B-B</t>
   </si>
   <si>
-    <t>See price in cart</t>
+    <t>NECJ044</t>
+  </si>
+  <si>
+    <t>AXM9718</t>
+  </si>
+  <si>
+    <t>IOG90EM</t>
+  </si>
+  <si>
+    <t>OCZT0WJ</t>
+  </si>
+  <si>
+    <t>http://www.zones.com/site/product/index.html?id=001598026</t>
+  </si>
+  <si>
+    <t>C7C95AW#ABA</t>
   </si>
 </sst>
 </file>
@@ -436,7 +452,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,8 +509,8 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
+      <c r="C6" s="1">
+        <v>345.99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -502,7 +518,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="1">
-        <v>1199</v>
+        <v>1249</v>
       </c>
     </row>
   </sheetData>
@@ -516,7 +532,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +585,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +630,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +672,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +693,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>714.99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -705,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +747,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="C2" s="1">
+        <v>34.99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -737,6 +759,53 @@
       </c>
       <c r="C3" s="1">
         <v>7845.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>106.25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>57.21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>21.17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>51.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>